<commit_message>
Added R2 and Alpha to output and changed model to Newey
</commit_message>
<xml_diff>
--- a/Regression Results/model_1_results.xlsx
+++ b/Regression Results/model_1_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,16 @@
           <t>Beta HML</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Alpha</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Adjusted R2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -485,13 +495,13 @@
         <v>-0.01265715199313849</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09073227398916023</v>
+        <v>0.1382729932387747</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.714215749458355</v>
+        <v>-1.482252984112642</v>
       </c>
       <c r="F2" t="n">
         <v>0.004830221386221036</v>
@@ -501,6 +511,12 @@
       </c>
       <c r="H2" t="n">
         <v>-1.068028738161389</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.004877181779817691</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.2453894587614225</v>
       </c>
     </row>
     <row r="3">
@@ -513,13 +529,13 @@
         <v>-0.005600166123145085</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5106761027157978</v>
+        <v>0.5359614640703878</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.6610266295366521</v>
+        <v>-0.6189315332752872</v>
       </c>
       <c r="F3" t="n">
         <v>-0.06822673757326753</v>
@@ -529,6 +545,12 @@
       </c>
       <c r="H3" t="n">
         <v>0.3772700717695266</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.0007364963197267401</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.01316497873353151</v>
       </c>
     </row>
     <row r="4">
@@ -541,13 +563,13 @@
         <v>0.01818051256686945</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05384932841325882</v>
+        <v>0.243460710302973</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1.959696806695702</v>
+        <v>1.166380323637777</v>
       </c>
       <c r="F4" t="n">
         <v>0.4550565778576708</v>
@@ -557,6 +579,12 @@
       </c>
       <c r="H4" t="n">
         <v>0.6665841414172906</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.002560966961518267</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.3764579905909564</v>
       </c>
     </row>
     <row r="5">
@@ -569,13 +597,13 @@
         <v>0.004884085774960451</v>
       </c>
       <c r="C5" t="n">
-        <v>0.652368499709401</v>
+        <v>0.5506088808635434</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4523357034627166</v>
+        <v>0.5968479800442473</v>
       </c>
       <c r="F5" t="n">
         <v>-0.3826888496060479</v>
@@ -585,6 +613,12 @@
       </c>
       <c r="H5" t="n">
         <v>0.6999413062949962</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-0.002121081048118593</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.257457228890327</v>
       </c>
     </row>
     <row r="6">
@@ -597,13 +631,13 @@
         <v>-0.06039696230683956</v>
       </c>
       <c r="C6" t="n">
-        <v>0.007429446036719514</v>
+        <v>0.1597896828439402</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.753818597172791</v>
+        <v>-1.405779258898873</v>
       </c>
       <c r="F6" t="n">
         <v>-0.6871886826415347</v>
@@ -613,6 +647,12 @@
       </c>
       <c r="H6" t="n">
         <v>-0.3783133081153229</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0112430145049063</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1540426079179317</v>
       </c>
     </row>
     <row r="7">
@@ -625,13 +665,13 @@
         <v>0.008432427610301758</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09340660602113024</v>
+        <v>0.1858576202422962</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1.699902770525991</v>
+        <v>1.322933119162968</v>
       </c>
       <c r="F7" t="n">
         <v>-0.05855988784450982</v>
@@ -641,6 +681,12 @@
       </c>
       <c r="H7" t="n">
         <v>0.4387418039263137</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.002138288787201321</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1556326995624852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>